<commit_message>
Done Cải tiến Kê thuốc
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Thuốc.xlsx
+++ b/DataTest/Data_API_Thuốc.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HIS api automation\DataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HIS api automation\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C01CCF-DD59-4EEC-B21A-83517779C2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85893756-C160-4726-BEFD-0BFC1CAEBF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="195">
   <si>
     <t>DxSymptom</t>
   </si>
@@ -73,9 +84,6 @@
     <t>ServiceId</t>
   </si>
   <si>
-    <t>Code1</t>
-  </si>
-  <si>
     <t>TypeL1</t>
   </si>
   <si>
@@ -464,13 +472,157 @@
   </si>
   <si>
     <t>Chiều: 1 Viên</t>
+  </si>
+  <si>
+    <t>RefNo</t>
+  </si>
+  <si>
+    <t>LabReqNotes</t>
+  </si>
+  <si>
+    <t>LabExId</t>
+  </si>
+  <si>
+    <t>MedServiceId</t>
+  </si>
+  <si>
+    <t>PriceId.1</t>
+  </si>
+  <si>
+    <t>InsPriceRatio</t>
+  </si>
+  <si>
+    <t>ByProviderId</t>
+  </si>
+  <si>
+    <t>DiscAmtSeq</t>
+  </si>
+  <si>
+    <t>MedServiceTypeL0</t>
+  </si>
+  <si>
+    <t>MedServiceTypeL2</t>
+  </si>
+  <si>
+    <t>MedServiceTypeL3</t>
+  </si>
+  <si>
+    <t>NonSubclinical</t>
+  </si>
+  <si>
+    <t>TypeL0Code</t>
+  </si>
+  <si>
+    <t>ByProviderCode</t>
+  </si>
+  <si>
+    <t>ByProviderName</t>
+  </si>
+  <si>
+    <t>ServiceGroupName.1</t>
+  </si>
+  <si>
+    <t>ServiceTypeL3Name</t>
+  </si>
+  <si>
+    <t>ServiceCode</t>
+  </si>
+  <si>
+    <t>ServiceName</t>
+  </si>
+  <si>
+    <t>InsBenefitTypeName</t>
+  </si>
+  <si>
+    <t>ReqDate</t>
+  </si>
+  <si>
+    <t>AttrString</t>
+  </si>
+  <si>
+    <t>PaidAttrString</t>
+  </si>
+  <si>
+    <t>ServiceTypeOrderIndex</t>
+  </si>
+  <si>
+    <t>MedItemType</t>
+  </si>
+  <si>
+    <t>MedItem</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>TotalInvoiceAmtRound</t>
+  </si>
+  <si>
+    <t>TotalReceiptAmtRound</t>
+  </si>
+  <si>
+    <t>PtAmt</t>
+  </si>
+  <si>
+    <t>PtAmtRound</t>
+  </si>
+  <si>
+    <t>PtAmtPaid</t>
+  </si>
+  <si>
+    <t>PtCoPayAmt</t>
+  </si>
+  <si>
+    <t>PtCoPayAmtRound</t>
+  </si>
+  <si>
+    <t>InsAmt</t>
+  </si>
+  <si>
+    <t>InsAmtRound</t>
+  </si>
+  <si>
+    <t>DiscAmt</t>
+  </si>
+  <si>
+    <t>ReqBy</t>
+  </si>
+  <si>
+    <t>FullAddress</t>
+  </si>
+  <si>
+    <t>Re</t>
+  </si>
+  <si>
+    <t>XQ1</t>
+  </si>
+  <si>
+    <t>Phòng X quang</t>
+  </si>
+  <si>
+    <t>Chẩn đoán hình ảnh</t>
+  </si>
+  <si>
+    <t>X-Quang</t>
+  </si>
+  <si>
+    <t>xq03</t>
+  </si>
+  <si>
+    <t>Chụp Xquang bể thận-niệu quản xuôi dòng [Số hóa]</t>
+  </si>
+  <si>
+    <t>BHYT</t>
+  </si>
+  <si>
+    <t>Chờ thanh toán</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +634,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -519,9 +677,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -826,441 +987,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DV2"/>
+  <dimension ref="A1:DV5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BG12" sqref="BG12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="46" max="46" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="42" customWidth="1"/>
+    <col min="38" max="38" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="15" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="33" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:126" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" s="1" t="s">
+      <c r="DL1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" s="1" t="s">
+      <c r="DP1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="DQ1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="DS1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="DT1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DV1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:126" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>126</v>
       </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
       <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
         <v>126</v>
       </c>
-      <c r="D2" t="s">
-        <v>127</v>
-      </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2">
         <v>3839</v>
@@ -1278,13 +1441,13 @@
         <v>17437</v>
       </c>
       <c r="O2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q2">
         <v>4803</v>
       </c>
       <c r="R2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S2">
         <v>13</v>
@@ -1305,13 +1468,13 @@
         <v>1</v>
       </c>
       <c r="Y2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z2" t="s">
         <v>130</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>131</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>132</v>
       </c>
       <c r="AB2">
         <v>1024</v>
@@ -1329,10 +1492,10 @@
         <v>37500</v>
       </c>
       <c r="AG2">
-        <v>1083660</v>
+        <v>1094172</v>
       </c>
       <c r="AK2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AL2">
         <v>0</v>
@@ -1356,10 +1519,10 @@
         <v>0</v>
       </c>
       <c r="BD2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="BE2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BF2">
         <v>2</v>
@@ -1380,13 +1543,13 @@
         <v>1</v>
       </c>
       <c r="BQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BU2" t="s">
         <v>138</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>135</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>139</v>
       </c>
       <c r="BV2">
         <v>1</v>
@@ -1395,25 +1558,25 @@
         <v>50</v>
       </c>
       <c r="BY2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CA2" t="s">
+        <v>138</v>
+      </c>
+      <c r="CB2" t="s">
         <v>139</v>
       </c>
-      <c r="CB2" t="s">
-        <v>140</v>
-      </c>
       <c r="CC2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="CD2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="CE2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="CG2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="CH2">
         <v>1</v>
@@ -1422,28 +1585,28 @@
         <v>1</v>
       </c>
       <c r="CJ2" t="s">
+        <v>140</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CO2" t="s">
         <v>141</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>138</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>142</v>
       </c>
       <c r="CP2">
         <v>242</v>
       </c>
       <c r="CQ2" t="s">
+        <v>142</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CS2" t="s">
         <v>143</v>
       </c>
-      <c r="CR2" t="s">
-        <v>136</v>
-      </c>
-      <c r="CS2" t="s">
+      <c r="CU2" t="s">
         <v>144</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>145</v>
       </c>
       <c r="CV2">
         <v>0</v>
@@ -1467,10 +1630,10 @@
         <v>1</v>
       </c>
       <c r="DE2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="DH2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="DI2" t="b">
         <v>0</v>
@@ -1482,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="DL2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="DM2" t="b">
         <v>1</v>
@@ -1491,7 +1654,452 @@
         <v>0</v>
       </c>
       <c r="DV2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:126" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM4" s="2" t="s">
         <v>147</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AV4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AW4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AX4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AY4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BA4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="BC4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="BD4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="BE4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="BH4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BI4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="BJ4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BK4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="BL4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="BM4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BN4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BO4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="BP4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BQ4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="BR4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="BS4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="BT4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="BU4" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="BV4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="BW4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="BX4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="BY4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="BZ4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="CA4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="CB4" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="CC4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="CD4" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:126" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5">
+        <v>3839</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>17437</v>
+      </c>
+      <c r="O5" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q5">
+        <v>4803</v>
+      </c>
+      <c r="R5" t="s">
+        <v>128</v>
+      </c>
+      <c r="S5">
+        <v>13</v>
+      </c>
+      <c r="T5">
+        <v>13</v>
+      </c>
+      <c r="U5">
+        <v>30</v>
+      </c>
+      <c r="V5">
+        <v>130</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB5">
+        <v>1024</v>
+      </c>
+      <c r="AC5">
+        <v>7.1897000000000002</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>37500</v>
+      </c>
+      <c r="AF5">
+        <v>37500</v>
+      </c>
+      <c r="AG5">
+        <v>1094172</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AL5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
+        <v>1</v>
+      </c>
+      <c r="AR5">
+        <v>382</v>
+      </c>
+      <c r="AS5">
+        <v>1095239</v>
+      </c>
+      <c r="AT5">
+        <v>1</v>
+      </c>
+      <c r="AU5">
+        <v>624000</v>
+      </c>
+      <c r="AV5">
+        <v>624000</v>
+      </c>
+      <c r="AW5">
+        <v>100</v>
+      </c>
+      <c r="AX5">
+        <v>552</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>2</v>
+      </c>
+      <c r="BA5">
+        <v>6</v>
+      </c>
+      <c r="BB5">
+        <v>25</v>
+      </c>
+      <c r="BC5" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>187</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>188</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>189</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>190</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>191</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>192</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>193</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>194</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>194</v>
+      </c>
+      <c r="BO5">
+        <v>0</v>
+      </c>
+      <c r="BP5">
+        <v>1</v>
+      </c>
+      <c r="BU5">
+        <v>0</v>
+      </c>
+      <c r="BV5">
+        <v>0</v>
+      </c>
+      <c r="BW5">
+        <v>0</v>
+      </c>
+      <c r="BX5">
+        <v>124800</v>
+      </c>
+      <c r="BY5">
+        <v>0</v>
+      </c>
+      <c r="BZ5">
+        <v>499200</v>
+      </c>
+      <c r="CA5">
+        <v>0</v>
+      </c>
+      <c r="CB5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>